<commit_message>
added dropdown for transaction type
</commit_message>
<xml_diff>
--- a/OTP_transaction_list.xlsx
+++ b/OTP_transaction_list.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -506,12 +506,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>m</t>
+          <t>q</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>rt</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>rtyj</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -540,6 +540,122 @@
         </is>
       </c>
       <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-08-06 09:48:30</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>malfoy</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>New Fitness Insception Receipt - 800</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>dobby</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1987d9a587a4073d</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-08-06 09:48:30</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>malfoy</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>New Reg &amp; MV Tax Receipt - xxxx</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>dobby</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>1987d9a587a4073d</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
 </t>

</xml_diff>

<commit_message>
adding pdf reading for rto receipts and reconciliation logic
</commit_message>
<xml_diff>
--- a/OTP_transaction_list.xlsx
+++ b/OTP_transaction_list.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
@@ -434,7 +434,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Timestamp</t>
+          <t>Transaction Date</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -656,6 +656,64 @@
         </is>
       </c>
       <c r="K4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-08-06 09:48:30</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5555</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>7777</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sirius</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Fitness Inspection Renewal - xxxx</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>kreacher</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>1987d9a587a4073d</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
 </t>

</xml_diff>

<commit_message>
fixed sync and downsync with googlesheets, added threading for downsync and otp fetch, transaction type refresh (based on sync and downsync)
</commit_message>
<xml_diff>
--- a/OTP_transaction_list.xlsx
+++ b/OTP_transaction_list.xlsx
@@ -2,14 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Transaction_Log" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Transaction_Types" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -412,24 +414,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <cols>
-    <col width="17.81640625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="18.1796875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="11.81640625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="12.54296875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="11.453125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="12.08984375" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="14.453125" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="17.1796875" bestFit="1" customWidth="1" min="9" max="10"/>
-    <col width="43.90625" bestFit="1" customWidth="1" min="11" max="11"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -491,232 +482,416 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>6 Aug 2025, 09:48</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MH14KQ3488</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>malfoy</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>National Permit Comm. Fee - 16500</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>dobby</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>1987d9a587a4073d</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>OTP for transaction amount of Rs1000 is 123456.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>2025-08-06 09:48:30</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>q</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>rt</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>"for testing"</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>990</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>1000</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>123456</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>rtyj</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>jklmnop</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
         <is>
           <t>1987d9a587a4073d</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>OTP for transaction amount of Rs1000 is 123456.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-08-06 09:48:30</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>qwerty</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>New Fitness Insception Receipt - 800</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>jklm</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>1987d9a587a4073d</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>OTP for transaction amount of Rs1000 is 123456.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-08-06 09:48:30</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>abcd</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Fresh Permit &amp; Authorisation Fee - 2500</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>huji</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>1987d9a587a4073d</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>OTP for transaction amount of Rs1000 is 123456.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-08-06 09:48:30</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Base Permit Renewal - xxxx</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1987d9a587a4073d</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>OTP for transaction amount of Rs1000 is 123456.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-08-06 09:48:30</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>New Reg &amp; MV Tax Receipt - xxxx</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1987d9a587a4073d</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
 </t>
         </is>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Transaction_Types</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>New Fitness Insception Receipt - 800</t>
+        </is>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-08-06 09:48:30</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>malfoy</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>New Fitness Insception Receipt - 800</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>990</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>dobby</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>1987d9a587a4073d</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
-</t>
+          <t>New Reg &amp; MV Tax Receipt - xxxx</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-08-06 09:48:30</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>malfoy</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>New Reg &amp; MV Tax Receipt - xxxx</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>990</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>dobby</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>1987d9a587a4073d</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
-</t>
+          <t>Fresh Permit &amp; Authorisation Fee - 2500</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-08-06 09:48:30</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5555</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>7777</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>sirius</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+          <t>National Permit Comm. Fee - 16500</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RC Particular - 50</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Fitness Inspection Renewal - xxxx</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>990</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>kreacher</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>1987d9a587a4073d</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">OTP for transaction amount of Rs1000 is 123456.
-</t>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MV Tax Renewal - 11500</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Authorisation NP - 1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Base Permit Renewal - xxxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hypo Termination - xxxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Hypo Endorsement - xxxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Transfer of Ownership - xxxx</t>
         </is>
       </c>
     </row>

</xml_diff>